<commit_message>
Added POM Structure. Added methods for Login Page for login and all other screens. Added 6 Test cases for each login page link
</commit_message>
<xml_diff>
--- a/TDDAutomationProject/src/main/java/com/qa/testdata/data.xlsx
+++ b/TDDAutomationProject/src/main/java/com/qa/testdata/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakeshrane/Tools/Test Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakeshrane/TDDAutomationFramework/TDDAutomationFramework/TDDAutomationProject/src/main/java/com/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,31 +27,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
-    <t>fw</t>
+    <t>Username</t>
   </si>
   <si>
-    <t>mngr119461</t>
+    <t>Password</t>
   </si>
   <si>
-    <t>bApazer</t>
-  </si>
-  <si>
-    <t>bapazer</t>
-  </si>
-  <si>
-    <t>mnGr119461</t>
-  </si>
-  <si>
-    <t>mnGr119461234</t>
+    <t>rakeshr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,6 +52,12 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -87,12 +84,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -372,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -380,67 +383,49 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>